<commit_message>
Interface board tests updated
</commit_message>
<xml_diff>
--- a/Interface board/PCB soldering and test/BoM and test procedure.xlsx
+++ b/Interface board/PCB soldering and test/BoM and test procedure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\estef\Documents\TFG\SemesterProjectPED2\Interface board\PCB soldering and test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{679B721F-A5DA-44D6-B39E-C4BB0259C193}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49BF7974-0977-4E12-8748-806195C3B782}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{060E8170-4DFF-46FB-89DA-8F0BC2815D53}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="282">
   <si>
     <t xml:space="preserve">BoM </t>
   </si>
@@ -175,9 +175,6 @@
     <t xml:space="preserve">5. Solder U6 </t>
   </si>
   <si>
-    <t xml:space="preserve">7. Check the LED light </t>
-  </si>
-  <si>
     <t xml:space="preserve">VS U7 </t>
   </si>
   <si>
@@ -202,9 +199,6 @@
     <t xml:space="preserve">1. Solder R46 </t>
   </si>
   <si>
-    <t xml:space="preserve">2. Solder C14,C15 </t>
-  </si>
-  <si>
     <t>3. Solder DS23</t>
   </si>
   <si>
@@ -221,15 +215,6 @@
   </si>
   <si>
     <t>4. Solder U7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5. Check the LED light </t>
-  </si>
-  <si>
-    <t>6. Apply 24V from external power supply in pins 1 and 2 (+Vin/-Vin) and measure it</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6. Apply 24V from external power supply in pins 1 and 2 (+Vin/GND) and measure it </t>
   </si>
   <si>
     <t>U6 and U8</t>
@@ -423,9 +408,6 @@
     <t xml:space="preserve">3. Solder U3-U5 </t>
   </si>
   <si>
-    <t xml:space="preserve">7. Measure with the multimeter the output voltage in pins 4 and 3 (+Vout/-Vout) for +15V </t>
-  </si>
-  <si>
     <t xml:space="preserve">DEBUGGING </t>
   </si>
   <si>
@@ -475,9 +457,6 @@
   </si>
   <si>
     <t xml:space="preserve">PASS/FAIL </t>
-  </si>
-  <si>
-    <t>6. Measure input voltage in pins 2 and 1 (+Vin/-Vin) for 5V (*The input is the output of U8)</t>
   </si>
   <si>
     <t>x</t>
@@ -761,12 +740,6 @@
     <t>*Matlab .m for the exact values expected --&gt; "Interface_board_calculations"</t>
   </si>
   <si>
-    <t xml:space="preserve">7. Check the temperature with the thermal camera </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6. Apply 24V to J22 and after apply 10V gradually up to 45V to J25 </t>
-  </si>
-  <si>
     <t xml:space="preserve">Operational amplifier </t>
   </si>
   <si>
@@ -782,12 +755,6 @@
     <t>4. Measure output voltage pin 1 (AD_36)</t>
   </si>
   <si>
-    <t xml:space="preserve">9. Check results with Matlab file </t>
-  </si>
-  <si>
-    <t>8. Measure the differential output (pin 7 and 6) but be careful! Do it in the resistors instead of the pins</t>
-  </si>
-  <si>
     <t xml:space="preserve">5. Check results with Matlab file </t>
   </si>
   <si>
@@ -843,13 +810,133 @@
   </si>
   <si>
     <t>5. Measure EncA_sig, EncB_sig, EncC_sig and it should be a square wave witn amplitude around 3.3V</t>
+  </si>
+  <si>
+    <t>7. Check the LED lights DS21 and DS25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. Apply 24V from external power supply in pins 1 and 2 (+Vin/-Vin) -&gt; J22 connector </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TRACO inputs were reversed so we cutted the trace and connected it correctly. </t>
+  </si>
+  <si>
+    <t>Vin=23.95V  Vout=13.62V</t>
+  </si>
+  <si>
+    <t>Vout = -13.62</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>2. Solder C12-C17</t>
+  </si>
+  <si>
+    <t>6. Apply 24V from external power supply in pins 1 and 2 (+Vin/GND)</t>
+  </si>
+  <si>
+    <t>7. Check the LED light DS23</t>
+  </si>
+  <si>
+    <t>5. Check the LED DS24</t>
+  </si>
+  <si>
+    <t>6. Measure input voltage in pins 2 and 1 (+Vin/-Vin) for 5V (*The input is the output of U8 so apply 24V)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7. Measure with the multimeter the output voltage in pins 4 and 3 (+Vout/-Vout) for +5V </t>
+  </si>
+  <si>
+    <t>R47 no connected anywhere</t>
+  </si>
+  <si>
+    <t>6. Solder J25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7. Apply 24V to J22 (for 5V VDD1,VDD2) and after apply 10V gradually up to 45V to J25 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8. Check the temperature with the thermal camera </t>
+  </si>
+  <si>
+    <t>9. Measure the differential output (pin 7 and 6) but be careful! Do it in the resistors instead of the pins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10. Check results with Matlab file </t>
+  </si>
+  <si>
+    <t>Sliders P1 and P2--&gt; 13,2-87,6K     14,5-91,6K</t>
+  </si>
+  <si>
+    <t>3 (they will be soldered later if we need them)</t>
+  </si>
+  <si>
+    <t>legs</t>
+  </si>
+  <si>
+    <t>10V</t>
+  </si>
+  <si>
+    <t>0,47V</t>
+  </si>
+  <si>
+    <t>15V</t>
+  </si>
+  <si>
+    <t>0,709V</t>
+  </si>
+  <si>
+    <t>20V</t>
+  </si>
+  <si>
+    <t>0,948 V</t>
+  </si>
+  <si>
+    <t>25V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,174V </t>
+  </si>
+  <si>
+    <t>30V</t>
+  </si>
+  <si>
+    <t>1,373V</t>
+  </si>
+  <si>
+    <t>40V</t>
+  </si>
+  <si>
+    <t>36V</t>
+  </si>
+  <si>
+    <t>23ºC</t>
+  </si>
+  <si>
+    <t>1,58V</t>
+  </si>
+  <si>
+    <t>30ºC</t>
+  </si>
+  <si>
+    <t>1,696 V</t>
+  </si>
+  <si>
+    <t>44V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,79V </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -908,8 +995,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -931,6 +1026,12 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -947,7 +1048,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -956,13 +1057,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -973,6 +1068,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
@@ -1290,43 +1394,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57855524-E3DC-48F2-8FAA-B0640212865A}">
-  <dimension ref="A1:I144"/>
+  <dimension ref="A1:K144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D137" sqref="D137"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H115" sqref="H115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.5546875" customWidth="1"/>
     <col min="2" max="2" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="84.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="90.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="70.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="G1" s="6" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="G1" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>19</v>
       </c>
@@ -1337,21 +1442,24 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H5" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1365,13 +1473,13 @@
         <v>33</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1387,8 +1495,11 @@
       <c r="G7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H7" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1404,31 +1515,46 @@
       <c r="G8" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H8" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C9" s="3"/>
       <c r="G9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H9" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C10" s="3"/>
       <c r="G10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="H10" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="J10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="3"/>
       <c r="G11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>243</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
@@ -1440,10 +1566,13 @@
         <v>30</v>
       </c>
       <c r="G12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <v>242</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1457,10 +1586,16 @@
         <v>34</v>
       </c>
       <c r="G13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="J13" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -1474,28 +1609,40 @@
         <v>36</v>
       </c>
       <c r="G14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="J14" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I15" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C16" s="3"/>
-      <c r="G16" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+      <c r="G16" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="3"/>
       <c r="G17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -1506,25 +1653,34 @@
         <v>5</v>
       </c>
       <c r="G18" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+        <v>249</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C19" s="3"/>
       <c r="G19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C20" s="3"/>
       <c r="G20" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H20" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1538,10 +1694,13 @@
         <v>30</v>
       </c>
       <c r="G21" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1555,10 +1714,13 @@
         <v>34</v>
       </c>
       <c r="G22" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+        <v>250</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1572,22 +1734,34 @@
         <v>36</v>
       </c>
       <c r="G23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+        <v>251</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C24" s="3"/>
       <c r="G24" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C25" s="3"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E25" t="s">
+        <v>263</v>
+      </c>
+      <c r="I25" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -1598,13 +1772,16 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>63</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -1615,18 +1792,24 @@
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>64</v>
+        <v>59</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
       </c>
       <c r="G27" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>15</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C28" s="3">
         <v>1</v>
@@ -1634,28 +1817,40 @@
       <c r="D28" t="s">
         <v>16</v>
       </c>
+      <c r="E28">
+        <v>3</v>
+      </c>
       <c r="G28" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>17</v>
       </c>
       <c r="B29" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C29" s="3">
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>67</v>
+        <v>62</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
       </c>
       <c r="G29" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -1666,39 +1861,54 @@
         <v>2</v>
       </c>
       <c r="D30" t="s">
-        <v>68</v>
+        <v>63</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
       </c>
       <c r="G30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G31" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+        <v>252</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G32" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+        <v>253</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G33" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+        <v>254</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>19</v>
       </c>
@@ -1709,424 +1919,478 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B38" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C38" s="3">
         <v>1</v>
       </c>
-      <c r="G38" s="5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G38" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B39" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C39" s="3">
         <v>1</v>
       </c>
       <c r="G39" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B40" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C40" s="3">
         <v>3</v>
       </c>
       <c r="D40" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G40" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C41" s="3"/>
       <c r="G41" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C42" s="3"/>
       <c r="G42" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C43" s="3"/>
       <c r="G43" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B44" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C44" s="3">
         <v>4</v>
       </c>
       <c r="D44" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G44" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B45" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C45" s="3">
         <v>4</v>
       </c>
       <c r="D45" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="I45" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>74</v>
+      </c>
+      <c r="B46" t="s">
         <v>79</v>
-      </c>
-      <c r="B46" t="s">
-        <v>84</v>
       </c>
       <c r="C46" s="3">
         <v>4</v>
       </c>
       <c r="D46" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B47" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C47" s="3">
         <v>4</v>
       </c>
       <c r="D47" t="s">
-        <v>90</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B48" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C48" s="3">
         <v>4</v>
       </c>
       <c r="D48" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G48" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B49" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C49" s="3">
         <v>12</v>
       </c>
       <c r="D49" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G49" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B50" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C50" s="3">
         <v>2</v>
       </c>
       <c r="D50" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G50" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G51" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C52" s="3"/>
       <c r="G52" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>11</v>
       </c>
       <c r="B53" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C53" s="3">
         <v>4</v>
       </c>
       <c r="D53" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G53" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C54" s="3">
         <v>4</v>
       </c>
       <c r="D54" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G54" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>11</v>
       </c>
       <c r="B55" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C55" s="3">
         <v>12</v>
       </c>
       <c r="D55" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G55" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G56" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C57" s="3"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>22</v>
       </c>
       <c r="B58" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C58" s="3">
         <v>4</v>
       </c>
       <c r="D58" t="s">
-        <v>100</v>
-      </c>
-      <c r="G58" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C59" s="3"/>
       <c r="G59" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C60" s="3"/>
       <c r="G60" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B61" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C61" s="3">
         <v>4</v>
       </c>
       <c r="D61" t="s">
-        <v>102</v>
+        <v>97</v>
+      </c>
+      <c r="E61">
+        <v>3</v>
       </c>
       <c r="G61" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B62" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C62" s="3">
         <v>2</v>
       </c>
       <c r="D62" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+      <c r="E62" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B63" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C63" s="3">
         <v>4</v>
       </c>
       <c r="D63" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="E63">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B64" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C64" s="3">
         <v>2</v>
       </c>
       <c r="D64" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+      <c r="E64" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B65" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C65" s="3">
         <v>3</v>
       </c>
       <c r="D65" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+      <c r="E65">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B66" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C66" s="3">
         <v>2</v>
       </c>
       <c r="D66" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+      <c r="E66">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A68" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B69" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C69" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B70" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C70" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A73" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="B73" s="4"/>
-      <c r="C73" s="4"/>
-      <c r="D73" s="4"/>
-      <c r="E73" s="4"/>
-      <c r="F73" s="4"/>
-      <c r="G73" s="4"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A73" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="B73" s="10"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="10"/>
+      <c r="F73" s="10"/>
+      <c r="G73" s="10"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
         <v>19</v>
       </c>
@@ -2137,202 +2401,217 @@
         <v>32</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A75" s="5" t="s">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A75" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C75" s="3"/>
-      <c r="G75" s="5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G75" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B76" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="C76" s="3">
         <v>6</v>
       </c>
       <c r="G76" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B77" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C77" s="3">
         <v>4</v>
       </c>
       <c r="D77" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G77" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C78" s="3"/>
       <c r="G78" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A79" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A79" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C79" s="3"/>
       <c r="G79" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>22</v>
       </c>
       <c r="B80" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C80" s="3">
         <v>4</v>
       </c>
       <c r="D80" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G80" t="s">
-        <v>174</v>
+        <v>167</v>
+      </c>
+      <c r="J80" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C81" s="3"/>
       <c r="G81" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A82" s="5" t="s">
+      <c r="A82" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C82" s="3"/>
+      <c r="E82" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C83" s="3"/>
       <c r="D83" t="s">
-        <v>150</v>
+        <v>143</v>
+      </c>
+      <c r="E83">
+        <v>3</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C84" s="3"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A85" s="5" t="s">
-        <v>117</v>
+      <c r="A85" s="4" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B86" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C86" s="3">
         <v>1</v>
       </c>
       <c r="D86" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B87" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C87" s="3">
         <v>1</v>
       </c>
       <c r="D87" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B88" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="C88" s="3">
         <v>1</v>
       </c>
       <c r="D88" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B89" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="C89" s="3">
         <v>1</v>
       </c>
       <c r="D89" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B90" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="C90" s="3">
         <v>1</v>
       </c>
       <c r="D90" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B91" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="C91" s="3">
         <v>1</v>
       </c>
       <c r="D91" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A93" s="5" t="s">
-        <v>165</v>
+      <c r="A93" s="4" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B94" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C94" s="3">
         <v>2</v>
@@ -2340,27 +2619,27 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B95" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C95" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A98" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="B98" s="4"/>
-      <c r="C98" s="4"/>
-      <c r="D98" s="4"/>
-      <c r="E98" s="4"/>
-      <c r="F98" s="4"/>
-      <c r="G98" s="4"/>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A98" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="B98" s="10"/>
+      <c r="C98" s="10"/>
+      <c r="D98" s="10"/>
+      <c r="E98" s="10"/>
+      <c r="F98" s="10"/>
+      <c r="G98" s="10"/>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B99" t="s">
         <v>19</v>
       </c>
@@ -2371,386 +2650,512 @@
         <v>32</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A100" s="5" t="s">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A100" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C100" s="3"/>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G100" s="8" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="B101" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C101" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G101" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>146</v>
-      </c>
-      <c r="B102" s="8" t="s">
-        <v>179</v>
+        <v>139</v>
+      </c>
+      <c r="B102" s="6" t="s">
+        <v>172</v>
       </c>
       <c r="C102" s="3">
         <v>8</v>
       </c>
-      <c r="G102" s="10" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G102" t="s">
+        <v>212</v>
+      </c>
+      <c r="H102" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="I102" t="s">
+        <v>264</v>
+      </c>
+      <c r="J102" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="B103" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="C103" s="3">
         <v>1</v>
       </c>
-      <c r="G103" s="5" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G103" t="s">
+        <v>213</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="I103" t="s">
+        <v>266</v>
+      </c>
+      <c r="J103" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B104" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C104" s="3">
         <v>2</v>
       </c>
       <c r="G104" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="I104" t="s">
+        <v>268</v>
+      </c>
+      <c r="J104" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="B105" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C105" s="3">
         <v>3</v>
       </c>
       <c r="G105" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+        <v>215</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="I105" t="s">
+        <v>270</v>
+      </c>
+      <c r="J105" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="B106" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C106" s="3">
         <v>1</v>
       </c>
       <c r="G106" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+        <v>216</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="I106" t="s">
+        <v>272</v>
+      </c>
+      <c r="J106" t="s">
+        <v>273</v>
+      </c>
+      <c r="K106" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="B107" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="C107" s="3">
         <v>3</v>
       </c>
       <c r="G107" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+        <v>256</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="I107" t="s">
+        <v>275</v>
+      </c>
+      <c r="J107" t="s">
+        <v>277</v>
+      </c>
+      <c r="K107" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B108" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C108" s="3">
         <v>3</v>
       </c>
       <c r="G108" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+        <v>257</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="I108" t="s">
+        <v>274</v>
+      </c>
+      <c r="J108" t="s">
+        <v>279</v>
+      </c>
+      <c r="K108">
+        <v>31.3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="B109" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="C109" s="3">
         <v>1</v>
       </c>
       <c r="G109" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="I109" t="s">
+        <v>280</v>
+      </c>
+      <c r="J109" t="s">
+        <v>281</v>
+      </c>
+      <c r="K109">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="B110" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="C110" s="3">
         <v>1</v>
       </c>
       <c r="G110" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G111" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A112" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="H111" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A112" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C112" s="3"/>
-      <c r="G112" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I112" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>22</v>
       </c>
-      <c r="B113" s="9" t="s">
-        <v>197</v>
+      <c r="B113" s="7" t="s">
+        <v>190</v>
       </c>
       <c r="C113" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="B114" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C114" s="3">
         <v>2</v>
       </c>
-      <c r="G114" s="5" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G114" s="4" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="B115" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C115" s="3">
         <v>1</v>
       </c>
       <c r="G115" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+        <v>219</v>
+      </c>
+      <c r="H115" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G116" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A117" s="5" t="s">
-        <v>202</v>
+        <v>220</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A117" s="4" t="s">
+        <v>195</v>
       </c>
       <c r="G117" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C118" s="2"/>
-      <c r="D118" s="10" t="s">
-        <v>205</v>
+      <c r="D118" s="8" t="s">
+        <v>198</v>
       </c>
       <c r="G118" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G119" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A120" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A120" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C120" s="3"/>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E120" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="B121" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C121" s="3">
         <v>1</v>
       </c>
       <c r="D121" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+      <c r="E121">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="C122" s="3">
         <v>1</v>
       </c>
       <c r="D122" t="s">
-        <v>210</v>
-      </c>
-      <c r="G122" s="5" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+      <c r="E122">
+        <v>3</v>
+      </c>
+      <c r="G122" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G123" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A124" s="5" t="s">
-        <v>211</v>
+        <v>225</v>
+      </c>
+      <c r="H123" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A124" s="4" t="s">
+        <v>204</v>
       </c>
       <c r="G124" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="B125" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C125" s="3">
         <v>1</v>
       </c>
       <c r="G125" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="B126" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="C126" s="3">
         <v>1</v>
       </c>
       <c r="D126" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="G126" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G128" s="4" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="129" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G129" t="s">
+        <v>229</v>
+      </c>
+      <c r="H129" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="130" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G130" t="s">
+        <v>230</v>
+      </c>
+      <c r="H130" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="131" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G131" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="132" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G132" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="134" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G134" s="4" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="135" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G135" t="s">
+        <v>233</v>
+      </c>
+      <c r="H135" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="136" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G136" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="137" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G137" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="139" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G139" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="140" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G140" t="s">
+        <v>237</v>
+      </c>
+      <c r="H140" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="141" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G141" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G128" s="5" t="s">
+      <c r="H141" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="142" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G142" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="129" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G129" t="s">
+    <row r="143" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G143" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="130" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G130" t="s">
+    <row r="144" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G144" t="s">
         <v>241</v>
-      </c>
-    </row>
-    <row r="131" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G131" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="132" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G132" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="134" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G134" s="5" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="135" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G135" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="136" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G136" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="137" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G137" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="139" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G139" s="5" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="140" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G140" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="141" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G141" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="142" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G142" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="143" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G143" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="144" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G144" t="s">
-        <v>252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>